<commit_message>
EOD 1 Mar - Pipeline finished to generate tables for form, rank and home/away - EDA and Modelling needed for next steps next week
</commit_message>
<xml_diff>
--- a/Excel Dataframes, EDA and Predictive Modelling/Bundesliga_Home_Away.xlsx
+++ b/Excel Dataframes, EDA and Predictive Modelling/Bundesliga_Home_Away.xlsx
@@ -426,7 +426,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I19"/>
+  <dimension ref="A1:R19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -480,6 +480,51 @@
           <t>PPG</t>
         </is>
       </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>S</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>SC</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>QS</t>
+        </is>
+      </c>
+      <c r="M1" s="1" t="inlineStr">
+        <is>
+          <t>QSC</t>
+        </is>
+      </c>
+      <c r="N1" s="1" t="inlineStr">
+        <is>
+          <t>BTTS%</t>
+        </is>
+      </c>
+      <c r="O1" s="1" t="inlineStr">
+        <is>
+          <t>Blank%</t>
+        </is>
+      </c>
+      <c r="P1" s="1" t="inlineStr">
+        <is>
+          <t>CS%</t>
+        </is>
+      </c>
+      <c r="Q1" s="1" t="inlineStr">
+        <is>
+          <t>FG%</t>
+        </is>
+      </c>
+      <c r="R1" s="1" t="inlineStr">
+        <is>
+          <t>FC%</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
@@ -511,6 +556,33 @@
       <c r="I2" t="n">
         <v>2.47</v>
       </c>
+      <c r="J2" t="n">
+        <v>287</v>
+      </c>
+      <c r="K2" t="n">
+        <v>145</v>
+      </c>
+      <c r="L2" t="n">
+        <v>53</v>
+      </c>
+      <c r="M2" t="n">
+        <v>23</v>
+      </c>
+      <c r="N2" t="n">
+        <v>0.59</v>
+      </c>
+      <c r="O2" t="n">
+        <v>0.06</v>
+      </c>
+      <c r="P2" t="n">
+        <v>0.41</v>
+      </c>
+      <c r="Q2" t="n">
+        <v>0.76</v>
+      </c>
+      <c r="R2" t="n">
+        <v>0.18</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
@@ -542,6 +614,33 @@
       <c r="I3" t="n">
         <v>2.44</v>
       </c>
+      <c r="J3" t="n">
+        <v>382</v>
+      </c>
+      <c r="K3" t="n">
+        <v>150</v>
+      </c>
+      <c r="L3" t="n">
+        <v>72</v>
+      </c>
+      <c r="M3" t="n">
+        <v>21</v>
+      </c>
+      <c r="N3" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="O3" t="n">
+        <v>0.06</v>
+      </c>
+      <c r="P3" t="n">
+        <v>0.44</v>
+      </c>
+      <c r="Q3" t="n">
+        <v>0.83</v>
+      </c>
+      <c r="R3" t="n">
+        <v>0.17</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="inlineStr">
@@ -573,6 +672,33 @@
       <c r="I4" t="n">
         <v>2.28</v>
       </c>
+      <c r="J4" t="n">
+        <v>304</v>
+      </c>
+      <c r="K4" t="n">
+        <v>186</v>
+      </c>
+      <c r="L4" t="n">
+        <v>46</v>
+      </c>
+      <c r="M4" t="n">
+        <v>28</v>
+      </c>
+      <c r="N4" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="O4" t="n">
+        <v>0.17</v>
+      </c>
+      <c r="P4" t="n">
+        <v>0.39</v>
+      </c>
+      <c r="Q4" t="n">
+        <v>0.67</v>
+      </c>
+      <c r="R4" t="n">
+        <v>0.28</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="inlineStr">
@@ -604,6 +730,33 @@
       <c r="I5" t="n">
         <v>2.17</v>
       </c>
+      <c r="J5" t="n">
+        <v>348</v>
+      </c>
+      <c r="K5" t="n">
+        <v>197</v>
+      </c>
+      <c r="L5" t="n">
+        <v>69</v>
+      </c>
+      <c r="M5" t="n">
+        <v>31</v>
+      </c>
+      <c r="N5" t="n">
+        <v>0.61</v>
+      </c>
+      <c r="O5" t="n">
+        <v>0.06</v>
+      </c>
+      <c r="P5" t="n">
+        <v>0.33</v>
+      </c>
+      <c r="Q5" t="n">
+        <v>0.72</v>
+      </c>
+      <c r="R5" t="n">
+        <v>0.28</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="inlineStr">
@@ -635,6 +788,33 @@
       <c r="I6" t="n">
         <v>2.06</v>
       </c>
+      <c r="J6" t="n">
+        <v>285</v>
+      </c>
+      <c r="K6" t="n">
+        <v>165</v>
+      </c>
+      <c r="L6" t="n">
+        <v>64</v>
+      </c>
+      <c r="M6" t="n">
+        <v>23</v>
+      </c>
+      <c r="N6" t="n">
+        <v>0.71</v>
+      </c>
+      <c r="O6" t="n">
+        <v>0.06</v>
+      </c>
+      <c r="P6" t="n">
+        <v>0.24</v>
+      </c>
+      <c r="Q6" t="n">
+        <v>0.59</v>
+      </c>
+      <c r="R6" t="n">
+        <v>0.41</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="inlineStr">
@@ -666,6 +846,33 @@
       <c r="I7" t="n">
         <v>1.82</v>
       </c>
+      <c r="J7" t="n">
+        <v>209</v>
+      </c>
+      <c r="K7" t="n">
+        <v>208</v>
+      </c>
+      <c r="L7" t="n">
+        <v>32</v>
+      </c>
+      <c r="M7" t="n">
+        <v>34</v>
+      </c>
+      <c r="N7" t="n">
+        <v>0.35</v>
+      </c>
+      <c r="O7" t="n">
+        <v>0.29</v>
+      </c>
+      <c r="P7" t="n">
+        <v>0.41</v>
+      </c>
+      <c r="Q7" t="n">
+        <v>0.59</v>
+      </c>
+      <c r="R7" t="n">
+        <v>0.35</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="inlineStr">
@@ -697,6 +904,33 @@
       <c r="I8" t="n">
         <v>1.76</v>
       </c>
+      <c r="J8" t="n">
+        <v>219</v>
+      </c>
+      <c r="K8" t="n">
+        <v>175</v>
+      </c>
+      <c r="L8" t="n">
+        <v>35</v>
+      </c>
+      <c r="M8" t="n">
+        <v>26</v>
+      </c>
+      <c r="N8" t="n">
+        <v>0.71</v>
+      </c>
+      <c r="O8" t="n">
+        <v>0.06</v>
+      </c>
+      <c r="P8" t="n">
+        <v>0.29</v>
+      </c>
+      <c r="Q8" t="n">
+        <v>0.53</v>
+      </c>
+      <c r="R8" t="n">
+        <v>0.41</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="inlineStr">
@@ -728,6 +962,33 @@
       <c r="I9" t="n">
         <v>1.71</v>
       </c>
+      <c r="J9" t="n">
+        <v>245</v>
+      </c>
+      <c r="K9" t="n">
+        <v>207</v>
+      </c>
+      <c r="L9" t="n">
+        <v>36</v>
+      </c>
+      <c r="M9" t="n">
+        <v>35</v>
+      </c>
+      <c r="N9" t="n">
+        <v>0.53</v>
+      </c>
+      <c r="O9" t="n">
+        <v>0.18</v>
+      </c>
+      <c r="P9" t="n">
+        <v>0.35</v>
+      </c>
+      <c r="Q9" t="n">
+        <v>0.53</v>
+      </c>
+      <c r="R9" t="n">
+        <v>0.41</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="inlineStr">
@@ -759,6 +1020,33 @@
       <c r="I10" t="n">
         <v>1.65</v>
       </c>
+      <c r="J10" t="n">
+        <v>268</v>
+      </c>
+      <c r="K10" t="n">
+        <v>269</v>
+      </c>
+      <c r="L10" t="n">
+        <v>42</v>
+      </c>
+      <c r="M10" t="n">
+        <v>30</v>
+      </c>
+      <c r="N10" t="n">
+        <v>0.76</v>
+      </c>
+      <c r="O10" t="n">
+        <v>0</v>
+      </c>
+      <c r="P10" t="n">
+        <v>0.24</v>
+      </c>
+      <c r="Q10" t="n">
+        <v>0.71</v>
+      </c>
+      <c r="R10" t="n">
+        <v>0.29</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="inlineStr">
@@ -790,6 +1078,33 @@
       <c r="I11" t="n">
         <v>1.65</v>
       </c>
+      <c r="J11" t="n">
+        <v>260</v>
+      </c>
+      <c r="K11" t="n">
+        <v>234</v>
+      </c>
+      <c r="L11" t="n">
+        <v>41</v>
+      </c>
+      <c r="M11" t="n">
+        <v>29</v>
+      </c>
+      <c r="N11" t="n">
+        <v>0.53</v>
+      </c>
+      <c r="O11" t="n">
+        <v>0.24</v>
+      </c>
+      <c r="P11" t="n">
+        <v>0.29</v>
+      </c>
+      <c r="Q11" t="n">
+        <v>0.71</v>
+      </c>
+      <c r="R11" t="n">
+        <v>0.24</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="inlineStr">
@@ -821,6 +1136,33 @@
       <c r="I12" t="n">
         <v>1.64</v>
       </c>
+      <c r="J12" t="n">
+        <v>153</v>
+      </c>
+      <c r="K12" t="n">
+        <v>160</v>
+      </c>
+      <c r="L12" t="n">
+        <v>15</v>
+      </c>
+      <c r="M12" t="n">
+        <v>23</v>
+      </c>
+      <c r="N12" t="n">
+        <v>0.64</v>
+      </c>
+      <c r="O12" t="n">
+        <v>0.18</v>
+      </c>
+      <c r="P12" t="n">
+        <v>0.36</v>
+      </c>
+      <c r="Q12" t="n">
+        <v>0.55</v>
+      </c>
+      <c r="R12" t="n">
+        <v>0.27</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="inlineStr">
@@ -852,6 +1194,33 @@
       <c r="I13" t="n">
         <v>1.47</v>
       </c>
+      <c r="J13" t="n">
+        <v>229</v>
+      </c>
+      <c r="K13" t="n">
+        <v>211</v>
+      </c>
+      <c r="L13" t="n">
+        <v>41</v>
+      </c>
+      <c r="M13" t="n">
+        <v>34</v>
+      </c>
+      <c r="N13" t="n">
+        <v>0.71</v>
+      </c>
+      <c r="O13" t="n">
+        <v>0.12</v>
+      </c>
+      <c r="P13" t="n">
+        <v>0.24</v>
+      </c>
+      <c r="Q13" t="n">
+        <v>0.41</v>
+      </c>
+      <c r="R13" t="n">
+        <v>0.53</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="inlineStr">
@@ -883,6 +1252,33 @@
       <c r="I14" t="n">
         <v>1.38</v>
       </c>
+      <c r="J14" t="n">
+        <v>230</v>
+      </c>
+      <c r="K14" t="n">
+        <v>215</v>
+      </c>
+      <c r="L14" t="n">
+        <v>32</v>
+      </c>
+      <c r="M14" t="n">
+        <v>36</v>
+      </c>
+      <c r="N14" t="n">
+        <v>0.88</v>
+      </c>
+      <c r="O14" t="n">
+        <v>0.06</v>
+      </c>
+      <c r="P14" t="n">
+        <v>0.06</v>
+      </c>
+      <c r="Q14" t="n">
+        <v>0.44</v>
+      </c>
+      <c r="R14" t="n">
+        <v>0.5600000000000001</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" s="1" t="inlineStr">
@@ -914,6 +1310,33 @@
       <c r="I15" t="n">
         <v>1.29</v>
       </c>
+      <c r="J15" t="n">
+        <v>195</v>
+      </c>
+      <c r="K15" t="n">
+        <v>248</v>
+      </c>
+      <c r="L15" t="n">
+        <v>27</v>
+      </c>
+      <c r="M15" t="n">
+        <v>39</v>
+      </c>
+      <c r="N15" t="n">
+        <v>0.82</v>
+      </c>
+      <c r="O15" t="n">
+        <v>0.12</v>
+      </c>
+      <c r="P15" t="n">
+        <v>0.06</v>
+      </c>
+      <c r="Q15" t="n">
+        <v>0.47</v>
+      </c>
+      <c r="R15" t="n">
+        <v>0.53</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16" s="1" t="inlineStr">
@@ -945,6 +1368,33 @@
       <c r="I16" t="n">
         <v>1.12</v>
       </c>
+      <c r="J16" t="n">
+        <v>206</v>
+      </c>
+      <c r="K16" t="n">
+        <v>211</v>
+      </c>
+      <c r="L16" t="n">
+        <v>31</v>
+      </c>
+      <c r="M16" t="n">
+        <v>34</v>
+      </c>
+      <c r="N16" t="n">
+        <v>0.71</v>
+      </c>
+      <c r="O16" t="n">
+        <v>0.12</v>
+      </c>
+      <c r="P16" t="n">
+        <v>0.18</v>
+      </c>
+      <c r="Q16" t="n">
+        <v>0.47</v>
+      </c>
+      <c r="R16" t="n">
+        <v>0.53</v>
+      </c>
     </row>
     <row r="17">
       <c r="A17" s="1" t="inlineStr">
@@ -976,6 +1426,33 @@
       <c r="I17" t="n">
         <v>0.88</v>
       </c>
+      <c r="J17" t="n">
+        <v>228</v>
+      </c>
+      <c r="K17" t="n">
+        <v>165</v>
+      </c>
+      <c r="L17" t="n">
+        <v>27</v>
+      </c>
+      <c r="M17" t="n">
+        <v>29</v>
+      </c>
+      <c r="N17" t="n">
+        <v>0.62</v>
+      </c>
+      <c r="O17" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="P17" t="n">
+        <v>0.12</v>
+      </c>
+      <c r="Q17" t="n">
+        <v>0.38</v>
+      </c>
+      <c r="R17" t="n">
+        <v>0.62</v>
+      </c>
     </row>
     <row r="18">
       <c r="A18" s="1" t="inlineStr">
@@ -1007,6 +1484,33 @@
       <c r="I18" t="n">
         <v>0.82</v>
       </c>
+      <c r="J18" t="n">
+        <v>258</v>
+      </c>
+      <c r="K18" t="n">
+        <v>198</v>
+      </c>
+      <c r="L18" t="n">
+        <v>21</v>
+      </c>
+      <c r="M18" t="n">
+        <v>42</v>
+      </c>
+      <c r="N18" t="n">
+        <v>0.47</v>
+      </c>
+      <c r="O18" t="n">
+        <v>0.47</v>
+      </c>
+      <c r="P18" t="n">
+        <v>0.18</v>
+      </c>
+      <c r="Q18" t="n">
+        <v>0.35</v>
+      </c>
+      <c r="R18" t="n">
+        <v>0.53</v>
+      </c>
     </row>
     <row r="19">
       <c r="A19" s="1" t="inlineStr">
@@ -1037,6 +1541,33 @@
       </c>
       <c r="I19" t="n">
         <v>0.5</v>
+      </c>
+      <c r="J19" t="n">
+        <v>169</v>
+      </c>
+      <c r="K19" t="n">
+        <v>156</v>
+      </c>
+      <c r="L19" t="n">
+        <v>19</v>
+      </c>
+      <c r="M19" t="n">
+        <v>31</v>
+      </c>
+      <c r="N19" t="n">
+        <v>0.58</v>
+      </c>
+      <c r="O19" t="n">
+        <v>0.42</v>
+      </c>
+      <c r="P19" t="n">
+        <v>0.08</v>
+      </c>
+      <c r="Q19" t="n">
+        <v>0.17</v>
+      </c>
+      <c r="R19" t="n">
+        <v>0.75</v>
       </c>
     </row>
   </sheetData>
@@ -1050,7 +1581,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I19"/>
+  <dimension ref="A1:R19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1104,6 +1635,51 @@
           <t>PPG</t>
         </is>
       </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>S</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>SC</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>QS</t>
+        </is>
+      </c>
+      <c r="M1" s="1" t="inlineStr">
+        <is>
+          <t>QSC</t>
+        </is>
+      </c>
+      <c r="N1" s="1" t="inlineStr">
+        <is>
+          <t>BTTS%</t>
+        </is>
+      </c>
+      <c r="O1" s="1" t="inlineStr">
+        <is>
+          <t>Blank%</t>
+        </is>
+      </c>
+      <c r="P1" s="1" t="inlineStr">
+        <is>
+          <t>CS%</t>
+        </is>
+      </c>
+      <c r="Q1" s="1" t="inlineStr">
+        <is>
+          <t>FG%</t>
+        </is>
+      </c>
+      <c r="R1" s="1" t="inlineStr">
+        <is>
+          <t>FC%</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
@@ -1135,6 +1711,33 @@
       <c r="I2" t="n">
         <v>2.24</v>
       </c>
+      <c r="J2" t="n">
+        <v>256</v>
+      </c>
+      <c r="K2" t="n">
+        <v>187</v>
+      </c>
+      <c r="L2" t="n">
+        <v>38</v>
+      </c>
+      <c r="M2" t="n">
+        <v>27</v>
+      </c>
+      <c r="N2" t="n">
+        <v>0.47</v>
+      </c>
+      <c r="O2" t="n">
+        <v>0.18</v>
+      </c>
+      <c r="P2" t="n">
+        <v>0.47</v>
+      </c>
+      <c r="Q2" t="n">
+        <v>0.53</v>
+      </c>
+      <c r="R2" t="n">
+        <v>0.35</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
@@ -1166,6 +1769,33 @@
       <c r="I3" t="n">
         <v>1.94</v>
       </c>
+      <c r="J3" t="n">
+        <v>268</v>
+      </c>
+      <c r="K3" t="n">
+        <v>171</v>
+      </c>
+      <c r="L3" t="n">
+        <v>52</v>
+      </c>
+      <c r="M3" t="n">
+        <v>21</v>
+      </c>
+      <c r="N3" t="n">
+        <v>0.6899999999999999</v>
+      </c>
+      <c r="O3" t="n">
+        <v>0.06</v>
+      </c>
+      <c r="P3" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="Q3" t="n">
+        <v>0.75</v>
+      </c>
+      <c r="R3" t="n">
+        <v>0.25</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="inlineStr">
@@ -1197,6 +1827,33 @@
       <c r="I4" t="n">
         <v>1.53</v>
       </c>
+      <c r="J4" t="n">
+        <v>220</v>
+      </c>
+      <c r="K4" t="n">
+        <v>203</v>
+      </c>
+      <c r="L4" t="n">
+        <v>45</v>
+      </c>
+      <c r="M4" t="n">
+        <v>29</v>
+      </c>
+      <c r="N4" t="n">
+        <v>0.65</v>
+      </c>
+      <c r="O4" t="n">
+        <v>0.24</v>
+      </c>
+      <c r="P4" t="n">
+        <v>0.12</v>
+      </c>
+      <c r="Q4" t="n">
+        <v>0.47</v>
+      </c>
+      <c r="R4" t="n">
+        <v>0.53</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="inlineStr">
@@ -1228,6 +1885,33 @@
       <c r="I5" t="n">
         <v>1.5</v>
       </c>
+      <c r="J5" t="n">
+        <v>233</v>
+      </c>
+      <c r="K5" t="n">
+        <v>235</v>
+      </c>
+      <c r="L5" t="n">
+        <v>46</v>
+      </c>
+      <c r="M5" t="n">
+        <v>36</v>
+      </c>
+      <c r="N5" t="n">
+        <v>0.75</v>
+      </c>
+      <c r="O5" t="n">
+        <v>0.06</v>
+      </c>
+      <c r="P5" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="Q5" t="n">
+        <v>0.62</v>
+      </c>
+      <c r="R5" t="n">
+        <v>0.31</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="inlineStr">
@@ -1259,6 +1943,33 @@
       <c r="I6" t="n">
         <v>1.44</v>
       </c>
+      <c r="J6" t="n">
+        <v>240</v>
+      </c>
+      <c r="K6" t="n">
+        <v>186</v>
+      </c>
+      <c r="L6" t="n">
+        <v>38</v>
+      </c>
+      <c r="M6" t="n">
+        <v>26</v>
+      </c>
+      <c r="N6" t="n">
+        <v>0.5600000000000001</v>
+      </c>
+      <c r="O6" t="n">
+        <v>0.19</v>
+      </c>
+      <c r="P6" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="Q6" t="n">
+        <v>0.44</v>
+      </c>
+      <c r="R6" t="n">
+        <v>0.5600000000000001</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="inlineStr">
@@ -1290,6 +2001,33 @@
       <c r="I7" t="n">
         <v>1.39</v>
       </c>
+      <c r="J7" t="n">
+        <v>197</v>
+      </c>
+      <c r="K7" t="n">
+        <v>308</v>
+      </c>
+      <c r="L7" t="n">
+        <v>31</v>
+      </c>
+      <c r="M7" t="n">
+        <v>39</v>
+      </c>
+      <c r="N7" t="n">
+        <v>0.83</v>
+      </c>
+      <c r="O7" t="n">
+        <v>0.11</v>
+      </c>
+      <c r="P7" t="n">
+        <v>0.06</v>
+      </c>
+      <c r="Q7" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="R7" t="n">
+        <v>0.5</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="inlineStr">
@@ -1321,6 +2059,33 @@
       <c r="I8" t="n">
         <v>1.06</v>
       </c>
+      <c r="J8" t="n">
+        <v>170</v>
+      </c>
+      <c r="K8" t="n">
+        <v>262</v>
+      </c>
+      <c r="L8" t="n">
+        <v>32</v>
+      </c>
+      <c r="M8" t="n">
+        <v>49</v>
+      </c>
+      <c r="N8" t="n">
+        <v>0.65</v>
+      </c>
+      <c r="O8" t="n">
+        <v>0.29</v>
+      </c>
+      <c r="P8" t="n">
+        <v>0.06</v>
+      </c>
+      <c r="Q8" t="n">
+        <v>0.53</v>
+      </c>
+      <c r="R8" t="n">
+        <v>0.47</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="inlineStr">
@@ -1352,6 +2117,33 @@
       <c r="I9" t="n">
         <v>1</v>
       </c>
+      <c r="J9" t="n">
+        <v>177</v>
+      </c>
+      <c r="K9" t="n">
+        <v>302</v>
+      </c>
+      <c r="L9" t="n">
+        <v>24</v>
+      </c>
+      <c r="M9" t="n">
+        <v>39</v>
+      </c>
+      <c r="N9" t="n">
+        <v>0.59</v>
+      </c>
+      <c r="O9" t="n">
+        <v>0.24</v>
+      </c>
+      <c r="P9" t="n">
+        <v>0.18</v>
+      </c>
+      <c r="Q9" t="n">
+        <v>0.47</v>
+      </c>
+      <c r="R9" t="n">
+        <v>0.53</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="inlineStr">
@@ -1383,6 +2175,33 @@
       <c r="I10" t="n">
         <v>1</v>
       </c>
+      <c r="J10" t="n">
+        <v>162</v>
+      </c>
+      <c r="K10" t="n">
+        <v>264</v>
+      </c>
+      <c r="L10" t="n">
+        <v>26</v>
+      </c>
+      <c r="M10" t="n">
+        <v>37</v>
+      </c>
+      <c r="N10" t="n">
+        <v>0.59</v>
+      </c>
+      <c r="O10" t="n">
+        <v>0.24</v>
+      </c>
+      <c r="P10" t="n">
+        <v>0.24</v>
+      </c>
+      <c r="Q10" t="n">
+        <v>0.47</v>
+      </c>
+      <c r="R10" t="n">
+        <v>0.47</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="inlineStr">
@@ -1414,6 +2233,33 @@
       <c r="I11" t="n">
         <v>0.88</v>
       </c>
+      <c r="J11" t="n">
+        <v>201</v>
+      </c>
+      <c r="K11" t="n">
+        <v>239</v>
+      </c>
+      <c r="L11" t="n">
+        <v>25</v>
+      </c>
+      <c r="M11" t="n">
+        <v>38</v>
+      </c>
+      <c r="N11" t="n">
+        <v>0.53</v>
+      </c>
+      <c r="O11" t="n">
+        <v>0.35</v>
+      </c>
+      <c r="P11" t="n">
+        <v>0.12</v>
+      </c>
+      <c r="Q11" t="n">
+        <v>0.47</v>
+      </c>
+      <c r="R11" t="n">
+        <v>0.53</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="inlineStr">
@@ -1445,6 +2291,33 @@
       <c r="I12" t="n">
         <v>0.88</v>
       </c>
+      <c r="J12" t="n">
+        <v>169</v>
+      </c>
+      <c r="K12" t="n">
+        <v>245</v>
+      </c>
+      <c r="L12" t="n">
+        <v>30</v>
+      </c>
+      <c r="M12" t="n">
+        <v>40</v>
+      </c>
+      <c r="N12" t="n">
+        <v>0.59</v>
+      </c>
+      <c r="O12" t="n">
+        <v>0.29</v>
+      </c>
+      <c r="P12" t="n">
+        <v>0.12</v>
+      </c>
+      <c r="Q12" t="n">
+        <v>0.29</v>
+      </c>
+      <c r="R12" t="n">
+        <v>0.71</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="inlineStr">
@@ -1476,6 +2349,33 @@
       <c r="I13" t="n">
         <v>0.83</v>
       </c>
+      <c r="J13" t="n">
+        <v>112</v>
+      </c>
+      <c r="K13" t="n">
+        <v>210</v>
+      </c>
+      <c r="L13" t="n">
+        <v>18</v>
+      </c>
+      <c r="M13" t="n">
+        <v>31</v>
+      </c>
+      <c r="N13" t="n">
+        <v>0.75</v>
+      </c>
+      <c r="O13" t="n">
+        <v>0.17</v>
+      </c>
+      <c r="P13" t="n">
+        <v>0.08</v>
+      </c>
+      <c r="Q13" t="n">
+        <v>0.33</v>
+      </c>
+      <c r="R13" t="n">
+        <v>0.67</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="inlineStr">
@@ -1507,6 +2407,33 @@
       <c r="I14" t="n">
         <v>0.76</v>
       </c>
+      <c r="J14" t="n">
+        <v>199</v>
+      </c>
+      <c r="K14" t="n">
+        <v>279</v>
+      </c>
+      <c r="L14" t="n">
+        <v>27</v>
+      </c>
+      <c r="M14" t="n">
+        <v>53</v>
+      </c>
+      <c r="N14" t="n">
+        <v>0.59</v>
+      </c>
+      <c r="O14" t="n">
+        <v>0.35</v>
+      </c>
+      <c r="P14" t="n">
+        <v>0.18</v>
+      </c>
+      <c r="Q14" t="n">
+        <v>0.24</v>
+      </c>
+      <c r="R14" t="n">
+        <v>0.65</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" s="1" t="inlineStr">
@@ -1538,6 +2465,33 @@
       <c r="I15" t="n">
         <v>0.71</v>
       </c>
+      <c r="J15" t="n">
+        <v>195</v>
+      </c>
+      <c r="K15" t="n">
+        <v>249</v>
+      </c>
+      <c r="L15" t="n">
+        <v>23</v>
+      </c>
+      <c r="M15" t="n">
+        <v>38</v>
+      </c>
+      <c r="N15" t="n">
+        <v>0.41</v>
+      </c>
+      <c r="O15" t="n">
+        <v>0.47</v>
+      </c>
+      <c r="P15" t="n">
+        <v>0.18</v>
+      </c>
+      <c r="Q15" t="n">
+        <v>0.24</v>
+      </c>
+      <c r="R15" t="n">
+        <v>0.71</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16" s="1" t="inlineStr">
@@ -1569,6 +2523,33 @@
       <c r="I16" t="n">
         <v>0.67</v>
       </c>
+      <c r="J16" t="n">
+        <v>201</v>
+      </c>
+      <c r="K16" t="n">
+        <v>245</v>
+      </c>
+      <c r="L16" t="n">
+        <v>29</v>
+      </c>
+      <c r="M16" t="n">
+        <v>39</v>
+      </c>
+      <c r="N16" t="n">
+        <v>0.61</v>
+      </c>
+      <c r="O16" t="n">
+        <v>0.33</v>
+      </c>
+      <c r="P16" t="n">
+        <v>0.17</v>
+      </c>
+      <c r="Q16" t="n">
+        <v>0.28</v>
+      </c>
+      <c r="R16" t="n">
+        <v>0.61</v>
+      </c>
     </row>
     <row r="17">
       <c r="A17" s="1" t="inlineStr">
@@ -1600,6 +2581,33 @@
       <c r="I17" t="n">
         <v>0.65</v>
       </c>
+      <c r="J17" t="n">
+        <v>198</v>
+      </c>
+      <c r="K17" t="n">
+        <v>266</v>
+      </c>
+      <c r="L17" t="n">
+        <v>24</v>
+      </c>
+      <c r="M17" t="n">
+        <v>46</v>
+      </c>
+      <c r="N17" t="n">
+        <v>0.65</v>
+      </c>
+      <c r="O17" t="n">
+        <v>0.35</v>
+      </c>
+      <c r="P17" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q17" t="n">
+        <v>0.24</v>
+      </c>
+      <c r="R17" t="n">
+        <v>0.76</v>
+      </c>
     </row>
     <row r="18">
       <c r="A18" s="1" t="inlineStr">
@@ -1631,6 +2639,33 @@
       <c r="I18" t="n">
         <v>0.64</v>
       </c>
+      <c r="J18" t="n">
+        <v>123</v>
+      </c>
+      <c r="K18" t="n">
+        <v>202</v>
+      </c>
+      <c r="L18" t="n">
+        <v>10</v>
+      </c>
+      <c r="M18" t="n">
+        <v>41</v>
+      </c>
+      <c r="N18" t="n">
+        <v>0.64</v>
+      </c>
+      <c r="O18" t="n">
+        <v>0.36</v>
+      </c>
+      <c r="P18" t="n">
+        <v>0.09</v>
+      </c>
+      <c r="Q18" t="n">
+        <v>0.27</v>
+      </c>
+      <c r="R18" t="n">
+        <v>0.64</v>
+      </c>
     </row>
     <row r="19">
       <c r="A19" s="1" t="inlineStr">
@@ -1661,6 +2696,33 @@
       </c>
       <c r="I19" t="n">
         <v>0.59</v>
+      </c>
+      <c r="J19" t="n">
+        <v>184</v>
+      </c>
+      <c r="K19" t="n">
+        <v>321</v>
+      </c>
+      <c r="L19" t="n">
+        <v>35</v>
+      </c>
+      <c r="M19" t="n">
+        <v>53</v>
+      </c>
+      <c r="N19" t="n">
+        <v>0.76</v>
+      </c>
+      <c r="O19" t="n">
+        <v>0.24</v>
+      </c>
+      <c r="P19" t="n">
+        <v>0.12</v>
+      </c>
+      <c r="Q19" t="n">
+        <v>0.35</v>
+      </c>
+      <c r="R19" t="n">
+        <v>0.53</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Gameweek update 5 March
</commit_message>
<xml_diff>
--- a/Excel Dataframes, EDA and Predictive Modelling/Bundesliga_Home_Away.xlsx
+++ b/Excel Dataframes, EDA and Predictive Modelling/Bundesliga_Home_Away.xlsx
@@ -591,55 +591,55 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C3" t="n">
-        <v>54.852</v>
+        <v>52.355</v>
       </c>
       <c r="D3" t="n">
-        <v>16.901</v>
+        <v>14.42</v>
       </c>
       <c r="E3" t="n">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="F3" t="n">
+        <v>14</v>
+      </c>
+      <c r="G3" t="n">
+        <v>39</v>
+      </c>
+      <c r="H3" t="n">
+        <v>41</v>
+      </c>
+      <c r="I3" t="n">
+        <v>2.41</v>
+      </c>
+      <c r="J3" t="n">
+        <v>359</v>
+      </c>
+      <c r="K3" t="n">
+        <v>137</v>
+      </c>
+      <c r="L3" t="n">
+        <v>70</v>
+      </c>
+      <c r="M3" t="n">
         <v>17</v>
       </c>
-      <c r="G3" t="n">
-        <v>41</v>
-      </c>
-      <c r="H3" t="n">
-        <v>44</v>
-      </c>
-      <c r="I3" t="n">
-        <v>2.44</v>
-      </c>
-      <c r="J3" t="n">
-        <v>382</v>
-      </c>
-      <c r="K3" t="n">
-        <v>150</v>
-      </c>
-      <c r="L3" t="n">
-        <v>72</v>
-      </c>
-      <c r="M3" t="n">
-        <v>21</v>
-      </c>
       <c r="N3" t="n">
-        <v>0.5</v>
+        <v>0.47</v>
       </c>
       <c r="O3" t="n">
         <v>0.06</v>
       </c>
       <c r="P3" t="n">
-        <v>0.44</v>
+        <v>0.47</v>
       </c>
       <c r="Q3" t="n">
-        <v>0.83</v>
+        <v>0.88</v>
       </c>
       <c r="R3" t="n">
-        <v>0.17</v>
+        <v>0.12</v>
       </c>
     </row>
     <row r="4">
@@ -649,55 +649,55 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C4" t="n">
-        <v>39.657</v>
+        <v>37.39</v>
       </c>
       <c r="D4" t="n">
-        <v>21.629</v>
+        <v>20.183</v>
       </c>
       <c r="E4" t="n">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="F4" t="n">
         <v>18</v>
       </c>
       <c r="G4" t="n">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="H4" t="n">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="I4" t="n">
-        <v>2.28</v>
+        <v>2.24</v>
       </c>
       <c r="J4" t="n">
-        <v>304</v>
+        <v>290</v>
       </c>
       <c r="K4" t="n">
-        <v>186</v>
+        <v>179</v>
       </c>
       <c r="L4" t="n">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="M4" t="n">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="N4" t="n">
-        <v>0.5</v>
+        <v>0.53</v>
       </c>
       <c r="O4" t="n">
-        <v>0.17</v>
+        <v>0.18</v>
       </c>
       <c r="P4" t="n">
-        <v>0.39</v>
+        <v>0.35</v>
       </c>
       <c r="Q4" t="n">
-        <v>0.67</v>
+        <v>0.65</v>
       </c>
       <c r="R4" t="n">
-        <v>0.28</v>
+        <v>0.29</v>
       </c>
     </row>
     <row r="5">
@@ -819,291 +819,291 @@
     <row r="7">
       <c r="A7" s="1" t="inlineStr">
         <is>
-          <t>Union Berlin</t>
+          <t>Eintracht Frankfurt</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C7" t="n">
-        <v>24.889</v>
+        <v>28.88</v>
       </c>
       <c r="D7" t="n">
-        <v>26.053</v>
+        <v>18.846</v>
       </c>
       <c r="E7" t="n">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="F7" t="n">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="G7" t="n">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="H7" t="n">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="I7" t="n">
-        <v>1.82</v>
+        <v>1.81</v>
       </c>
       <c r="J7" t="n">
         <v>209</v>
       </c>
       <c r="K7" t="n">
-        <v>208</v>
+        <v>165</v>
       </c>
       <c r="L7" t="n">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="M7" t="n">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="N7" t="n">
-        <v>0.35</v>
+        <v>0.6899999999999999</v>
       </c>
       <c r="O7" t="n">
-        <v>0.29</v>
+        <v>0.06</v>
       </c>
       <c r="P7" t="n">
-        <v>0.41</v>
+        <v>0.31</v>
       </c>
       <c r="Q7" t="n">
-        <v>0.59</v>
+        <v>0.5</v>
       </c>
       <c r="R7" t="n">
-        <v>0.35</v>
+        <v>0.44</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="inlineStr">
         <is>
-          <t>Eintracht Frankfurt</t>
+          <t>Union Berlin</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C8" t="n">
-        <v>29.407</v>
+        <v>25.92</v>
       </c>
       <c r="D8" t="n">
-        <v>19.28</v>
+        <v>27.703</v>
       </c>
       <c r="E8" t="n">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="F8" t="n">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="G8" t="n">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="H8" t="n">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="I8" t="n">
-        <v>1.76</v>
+        <v>1.72</v>
       </c>
       <c r="J8" t="n">
-        <v>219</v>
+        <v>223</v>
       </c>
       <c r="K8" t="n">
-        <v>175</v>
+        <v>221</v>
       </c>
       <c r="L8" t="n">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="M8" t="n">
-        <v>26</v>
+        <v>36</v>
       </c>
       <c r="N8" t="n">
-        <v>0.71</v>
+        <v>0.33</v>
       </c>
       <c r="O8" t="n">
-        <v>0.06</v>
+        <v>0.33</v>
       </c>
       <c r="P8" t="n">
-        <v>0.29</v>
+        <v>0.39</v>
       </c>
       <c r="Q8" t="n">
-        <v>0.53</v>
+        <v>0.5600000000000001</v>
       </c>
       <c r="R8" t="n">
-        <v>0.41</v>
+        <v>0.39</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="inlineStr">
         <is>
-          <t>Freiburg</t>
+          <t>Borussia M.Gladbach</t>
         </is>
       </c>
       <c r="B9" t="n">
         <v>17</v>
       </c>
       <c r="C9" t="n">
-        <v>30.815</v>
+        <v>32.299</v>
       </c>
       <c r="D9" t="n">
-        <v>25.731</v>
+        <v>22.476</v>
       </c>
       <c r="E9" t="n">
+        <v>30</v>
+      </c>
+      <c r="F9" t="n">
+        <v>20</v>
+      </c>
+      <c r="G9" t="n">
+        <v>10</v>
+      </c>
+      <c r="H9" t="n">
+        <v>28</v>
+      </c>
+      <c r="I9" t="n">
+        <v>1.65</v>
+      </c>
+      <c r="J9" t="n">
+        <v>260</v>
+      </c>
+      <c r="K9" t="n">
+        <v>234</v>
+      </c>
+      <c r="L9" t="n">
+        <v>41</v>
+      </c>
+      <c r="M9" t="n">
         <v>29</v>
-      </c>
-      <c r="F9" t="n">
-        <v>21</v>
-      </c>
-      <c r="G9" t="n">
-        <v>8</v>
-      </c>
-      <c r="H9" t="n">
-        <v>29</v>
-      </c>
-      <c r="I9" t="n">
-        <v>1.71</v>
-      </c>
-      <c r="J9" t="n">
-        <v>245</v>
-      </c>
-      <c r="K9" t="n">
-        <v>207</v>
-      </c>
-      <c r="L9" t="n">
-        <v>36</v>
-      </c>
-      <c r="M9" t="n">
-        <v>35</v>
       </c>
       <c r="N9" t="n">
         <v>0.53</v>
       </c>
       <c r="O9" t="n">
-        <v>0.18</v>
+        <v>0.24</v>
       </c>
       <c r="P9" t="n">
-        <v>0.35</v>
+        <v>0.29</v>
       </c>
       <c r="Q9" t="n">
-        <v>0.53</v>
+        <v>0.71</v>
       </c>
       <c r="R9" t="n">
-        <v>0.41</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="inlineStr">
         <is>
-          <t>Bochum</t>
+          <t>Freiburg</t>
         </is>
       </c>
       <c r="B10" t="n">
         <v>17</v>
       </c>
       <c r="C10" t="n">
-        <v>33.395</v>
+        <v>31.968</v>
       </c>
       <c r="D10" t="n">
-        <v>29.412</v>
+        <v>27.012</v>
       </c>
       <c r="E10" t="n">
         <v>29</v>
       </c>
       <c r="F10" t="n">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="G10" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="H10" t="n">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="I10" t="n">
-        <v>1.65</v>
+        <v>1.59</v>
       </c>
       <c r="J10" t="n">
-        <v>268</v>
+        <v>253</v>
       </c>
       <c r="K10" t="n">
-        <v>269</v>
+        <v>215</v>
       </c>
       <c r="L10" t="n">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="M10" t="n">
-        <v>30</v>
+        <v>38</v>
       </c>
       <c r="N10" t="n">
-        <v>0.76</v>
+        <v>0.53</v>
       </c>
       <c r="O10" t="n">
-        <v>0</v>
+        <v>0.18</v>
       </c>
       <c r="P10" t="n">
-        <v>0.24</v>
+        <v>0.35</v>
       </c>
       <c r="Q10" t="n">
-        <v>0.71</v>
+        <v>0.53</v>
       </c>
       <c r="R10" t="n">
-        <v>0.29</v>
+        <v>0.41</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="inlineStr">
         <is>
-          <t>Borussia M.Gladbach</t>
+          <t>Bochum</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C11" t="n">
-        <v>32.299</v>
+        <v>33.958</v>
       </c>
       <c r="D11" t="n">
-        <v>22.476</v>
+        <v>31.529</v>
       </c>
       <c r="E11" t="n">
         <v>30</v>
       </c>
       <c r="F11" t="n">
-        <v>20</v>
+        <v>28</v>
       </c>
       <c r="G11" t="n">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="H11" t="n">
         <v>28</v>
       </c>
       <c r="I11" t="n">
-        <v>1.65</v>
+        <v>1.56</v>
       </c>
       <c r="J11" t="n">
-        <v>260</v>
+        <v>283</v>
       </c>
       <c r="K11" t="n">
-        <v>234</v>
+        <v>281</v>
       </c>
       <c r="L11" t="n">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="M11" t="n">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="N11" t="n">
-        <v>0.53</v>
+        <v>0.78</v>
       </c>
       <c r="O11" t="n">
-        <v>0.24</v>
+        <v>0</v>
       </c>
       <c r="P11" t="n">
-        <v>0.29</v>
+        <v>0.22</v>
       </c>
       <c r="Q11" t="n">
-        <v>0.71</v>
+        <v>0.72</v>
       </c>
       <c r="R11" t="n">
-        <v>0.24</v>
+        <v>0.28</v>
       </c>
     </row>
     <row r="12">
@@ -1113,80 +1113,80 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C12" t="n">
-        <v>15.35</v>
+        <v>16.198</v>
       </c>
       <c r="D12" t="n">
-        <v>20.612</v>
+        <v>22.307</v>
       </c>
       <c r="E12" t="n">
+        <v>20</v>
+      </c>
+      <c r="F12" t="n">
         <v>19</v>
       </c>
-      <c r="F12" t="n">
-        <v>17</v>
-      </c>
       <c r="G12" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H12" t="n">
         <v>18</v>
       </c>
       <c r="I12" t="n">
-        <v>1.64</v>
+        <v>1.5</v>
       </c>
       <c r="J12" t="n">
-        <v>153</v>
+        <v>169</v>
       </c>
       <c r="K12" t="n">
-        <v>160</v>
+        <v>170</v>
       </c>
       <c r="L12" t="n">
         <v>15</v>
       </c>
       <c r="M12" t="n">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="N12" t="n">
-        <v>0.64</v>
+        <v>0.67</v>
       </c>
       <c r="O12" t="n">
-        <v>0.18</v>
+        <v>0.17</v>
       </c>
       <c r="P12" t="n">
-        <v>0.36</v>
+        <v>0.33</v>
       </c>
       <c r="Q12" t="n">
-        <v>0.55</v>
+        <v>0.5</v>
       </c>
       <c r="R12" t="n">
-        <v>0.27</v>
+        <v>0.33</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="inlineStr">
         <is>
-          <t>Wolfsburg</t>
+          <t>Hoffenheim</t>
         </is>
       </c>
       <c r="B13" t="n">
         <v>17</v>
       </c>
       <c r="C13" t="n">
-        <v>29.998</v>
+        <v>31.23</v>
       </c>
       <c r="D13" t="n">
-        <v>24.658</v>
+        <v>26.839</v>
       </c>
       <c r="E13" t="n">
-        <v>25</v>
+        <v>32</v>
       </c>
       <c r="F13" t="n">
-        <v>19</v>
+        <v>28</v>
       </c>
       <c r="G13" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="H13" t="n">
         <v>25</v>
@@ -1195,28 +1195,28 @@
         <v>1.47</v>
       </c>
       <c r="J13" t="n">
-        <v>229</v>
+        <v>244</v>
       </c>
       <c r="K13" t="n">
-        <v>211</v>
+        <v>233</v>
       </c>
       <c r="L13" t="n">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="M13" t="n">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="N13" t="n">
-        <v>0.71</v>
+        <v>0.88</v>
       </c>
       <c r="O13" t="n">
-        <v>0.12</v>
+        <v>0.06</v>
       </c>
       <c r="P13" t="n">
-        <v>0.24</v>
+        <v>0.06</v>
       </c>
       <c r="Q13" t="n">
-        <v>0.41</v>
+        <v>0.47</v>
       </c>
       <c r="R13" t="n">
         <v>0.53</v>
@@ -1225,59 +1225,59 @@
     <row r="14">
       <c r="A14" s="1" t="inlineStr">
         <is>
-          <t>Hoffenheim</t>
+          <t>Wolfsburg</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C14" t="n">
-        <v>29.164</v>
+        <v>29.65</v>
       </c>
       <c r="D14" t="n">
-        <v>25.49</v>
+        <v>24.473</v>
       </c>
       <c r="E14" t="n">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="F14" t="n">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="G14" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="H14" t="n">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="I14" t="n">
-        <v>1.38</v>
+        <v>1.41</v>
       </c>
       <c r="J14" t="n">
-        <v>230</v>
+        <v>226</v>
       </c>
       <c r="K14" t="n">
-        <v>215</v>
+        <v>206</v>
       </c>
       <c r="L14" t="n">
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="M14" t="n">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="N14" t="n">
-        <v>0.88</v>
+        <v>0.71</v>
       </c>
       <c r="O14" t="n">
-        <v>0.06</v>
+        <v>0.12</v>
       </c>
       <c r="P14" t="n">
-        <v>0.06</v>
+        <v>0.24</v>
       </c>
       <c r="Q14" t="n">
-        <v>0.44</v>
+        <v>0.41</v>
       </c>
       <c r="R14" t="n">
-        <v>0.5600000000000001</v>
+        <v>0.53</v>
       </c>
     </row>
     <row r="15">
@@ -1345,55 +1345,55 @@
         </is>
       </c>
       <c r="B16" t="n">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C16" t="n">
-        <v>24.728</v>
+        <v>23.02</v>
       </c>
       <c r="D16" t="n">
-        <v>25.971</v>
+        <v>24.753</v>
       </c>
       <c r="E16" t="n">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="F16" t="n">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="G16" t="n">
-        <v>-2</v>
+        <v>-1</v>
       </c>
       <c r="H16" t="n">
         <v>19</v>
       </c>
       <c r="I16" t="n">
-        <v>1.12</v>
+        <v>1.19</v>
       </c>
       <c r="J16" t="n">
-        <v>206</v>
+        <v>194</v>
       </c>
       <c r="K16" t="n">
-        <v>211</v>
+        <v>197</v>
       </c>
       <c r="L16" t="n">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="M16" t="n">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="N16" t="n">
-        <v>0.71</v>
+        <v>0.6899999999999999</v>
       </c>
       <c r="O16" t="n">
         <v>0.12</v>
       </c>
       <c r="P16" t="n">
-        <v>0.18</v>
+        <v>0.19</v>
       </c>
       <c r="Q16" t="n">
-        <v>0.47</v>
+        <v>0.44</v>
       </c>
       <c r="R16" t="n">
-        <v>0.53</v>
+        <v>0.5600000000000001</v>
       </c>
     </row>
     <row r="17">
@@ -1403,55 +1403,55 @@
         </is>
       </c>
       <c r="B17" t="n">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C17" t="n">
-        <v>22.519</v>
+        <v>23.608</v>
       </c>
       <c r="D17" t="n">
-        <v>21.009</v>
+        <v>22.56</v>
       </c>
       <c r="E17" t="n">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="F17" t="n">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="G17" t="n">
         <v>-9</v>
       </c>
       <c r="H17" t="n">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="I17" t="n">
         <v>0.88</v>
       </c>
       <c r="J17" t="n">
-        <v>228</v>
+        <v>247</v>
       </c>
       <c r="K17" t="n">
-        <v>165</v>
+        <v>179</v>
       </c>
       <c r="L17" t="n">
         <v>27</v>
       </c>
       <c r="M17" t="n">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="N17" t="n">
-        <v>0.62</v>
+        <v>0.65</v>
       </c>
       <c r="O17" t="n">
-        <v>0.25</v>
+        <v>0.24</v>
       </c>
       <c r="P17" t="n">
         <v>0.12</v>
       </c>
       <c r="Q17" t="n">
-        <v>0.38</v>
+        <v>0.41</v>
       </c>
       <c r="R17" t="n">
-        <v>0.62</v>
+        <v>0.59</v>
       </c>
     </row>
     <row r="18">
@@ -1464,10 +1464,10 @@
         <v>17</v>
       </c>
       <c r="C18" t="n">
-        <v>22.905</v>
+        <v>23.614</v>
       </c>
       <c r="D18" t="n">
-        <v>29.677</v>
+        <v>29.64</v>
       </c>
       <c r="E18" t="n">
         <v>16</v>
@@ -1485,16 +1485,16 @@
         <v>0.82</v>
       </c>
       <c r="J18" t="n">
-        <v>258</v>
+        <v>253</v>
       </c>
       <c r="K18" t="n">
-        <v>198</v>
+        <v>206</v>
       </c>
       <c r="L18" t="n">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="M18" t="n">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="N18" t="n">
         <v>0.47</v>
@@ -1519,55 +1519,55 @@
         </is>
       </c>
       <c r="B19" t="n">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C19" t="n">
-        <v>16.26</v>
+        <v>17.374</v>
       </c>
       <c r="D19" t="n">
-        <v>21.072</v>
+        <v>24.468</v>
       </c>
       <c r="E19" t="n">
         <v>13</v>
       </c>
       <c r="F19" t="n">
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="G19" t="n">
-        <v>-12</v>
+        <v>-18</v>
       </c>
       <c r="H19" t="n">
         <v>6</v>
       </c>
       <c r="I19" t="n">
-        <v>0.5</v>
+        <v>0.46</v>
       </c>
       <c r="J19" t="n">
-        <v>169</v>
+        <v>179</v>
       </c>
       <c r="K19" t="n">
-        <v>156</v>
+        <v>178</v>
       </c>
       <c r="L19" t="n">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="M19" t="n">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="N19" t="n">
-        <v>0.58</v>
+        <v>0.54</v>
       </c>
       <c r="O19" t="n">
-        <v>0.42</v>
+        <v>0.46</v>
       </c>
       <c r="P19" t="n">
         <v>0.08</v>
       </c>
       <c r="Q19" t="n">
-        <v>0.17</v>
+        <v>0.15</v>
       </c>
       <c r="R19" t="n">
-        <v>0.75</v>
+        <v>0.77</v>
       </c>
     </row>
   </sheetData>
@@ -1691,19 +1691,19 @@
         <v>17</v>
       </c>
       <c r="C2" t="n">
-        <v>30.547</v>
+        <v>31.026</v>
       </c>
       <c r="D2" t="n">
-        <v>20.759</v>
+        <v>20.345</v>
       </c>
       <c r="E2" t="n">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F2" t="n">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="G2" t="n">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="H2" t="n">
         <v>38</v>
@@ -1712,31 +1712,31 @@
         <v>2.24</v>
       </c>
       <c r="J2" t="n">
-        <v>256</v>
+        <v>259</v>
       </c>
       <c r="K2" t="n">
-        <v>187</v>
+        <v>181</v>
       </c>
       <c r="L2" t="n">
         <v>38</v>
       </c>
       <c r="M2" t="n">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="N2" t="n">
-        <v>0.47</v>
+        <v>0.41</v>
       </c>
       <c r="O2" t="n">
         <v>0.18</v>
       </c>
       <c r="P2" t="n">
-        <v>0.47</v>
+        <v>0.53</v>
       </c>
       <c r="Q2" t="n">
-        <v>0.53</v>
+        <v>0.59</v>
       </c>
       <c r="R2" t="n">
-        <v>0.35</v>
+        <v>0.29</v>
       </c>
     </row>
     <row r="3">
@@ -1746,55 +1746,55 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C3" t="n">
-        <v>38.096</v>
+        <v>40.538</v>
       </c>
       <c r="D3" t="n">
-        <v>18.664</v>
+        <v>20.269</v>
       </c>
       <c r="E3" t="n">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="F3" t="n">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="G3" t="n">
         <v>6</v>
       </c>
       <c r="H3" t="n">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="I3" t="n">
-        <v>1.94</v>
+        <v>1.88</v>
       </c>
       <c r="J3" t="n">
-        <v>268</v>
+        <v>288</v>
       </c>
       <c r="K3" t="n">
-        <v>171</v>
+        <v>188</v>
       </c>
       <c r="L3" t="n">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="M3" t="n">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="N3" t="n">
-        <v>0.6899999999999999</v>
+        <v>0.71</v>
       </c>
       <c r="O3" t="n">
         <v>0.06</v>
       </c>
       <c r="P3" t="n">
-        <v>0.25</v>
+        <v>0.24</v>
       </c>
       <c r="Q3" t="n">
-        <v>0.75</v>
+        <v>0.71</v>
       </c>
       <c r="R3" t="n">
-        <v>0.25</v>
+        <v>0.29</v>
       </c>
     </row>
     <row r="4">
@@ -1807,34 +1807,34 @@
         <v>17</v>
       </c>
       <c r="C4" t="n">
-        <v>30.195</v>
+        <v>30.802</v>
       </c>
       <c r="D4" t="n">
-        <v>24.412</v>
+        <v>24.869</v>
       </c>
       <c r="E4" t="n">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="F4" t="n">
+        <v>29</v>
+      </c>
+      <c r="G4" t="n">
+        <v>0</v>
+      </c>
+      <c r="H4" t="n">
         <v>28</v>
       </c>
-      <c r="G4" t="n">
-        <v>-1</v>
-      </c>
-      <c r="H4" t="n">
-        <v>26</v>
-      </c>
       <c r="I4" t="n">
-        <v>1.53</v>
+        <v>1.65</v>
       </c>
       <c r="J4" t="n">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="K4" t="n">
-        <v>203</v>
+        <v>205</v>
       </c>
       <c r="L4" t="n">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="M4" t="n">
         <v>29</v>
@@ -1849,10 +1849,10 @@
         <v>0.12</v>
       </c>
       <c r="Q4" t="n">
+        <v>0.53</v>
+      </c>
+      <c r="R4" t="n">
         <v>0.47</v>
-      </c>
-      <c r="R4" t="n">
-        <v>0.53</v>
       </c>
     </row>
     <row r="5">
@@ -1865,46 +1865,46 @@
         <v>16</v>
       </c>
       <c r="C5" t="n">
-        <v>33.448</v>
+        <v>33.876</v>
       </c>
       <c r="D5" t="n">
-        <v>28.597</v>
+        <v>28.103</v>
       </c>
       <c r="E5" t="n">
         <v>33</v>
       </c>
       <c r="F5" t="n">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="G5" t="n">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="H5" t="n">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="I5" t="n">
-        <v>1.5</v>
+        <v>1.62</v>
       </c>
       <c r="J5" t="n">
-        <v>233</v>
+        <v>227</v>
       </c>
       <c r="K5" t="n">
-        <v>235</v>
+        <v>239</v>
       </c>
       <c r="L5" t="n">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="M5" t="n">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="N5" t="n">
-        <v>0.75</v>
+        <v>0.6899999999999999</v>
       </c>
       <c r="O5" t="n">
         <v>0.06</v>
       </c>
       <c r="P5" t="n">
-        <v>0.25</v>
+        <v>0.31</v>
       </c>
       <c r="Q5" t="n">
         <v>0.62</v>
@@ -1920,55 +1920,55 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C6" t="n">
-        <v>29.633</v>
+        <v>31.75</v>
       </c>
       <c r="D6" t="n">
-        <v>20.53</v>
+        <v>21.093</v>
       </c>
       <c r="E6" t="n">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="F6" t="n">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="G6" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H6" t="n">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="I6" t="n">
-        <v>1.44</v>
+        <v>1.53</v>
       </c>
       <c r="J6" t="n">
-        <v>240</v>
+        <v>252</v>
       </c>
       <c r="K6" t="n">
-        <v>186</v>
+        <v>201</v>
       </c>
       <c r="L6" t="n">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="M6" t="n">
         <v>26</v>
       </c>
       <c r="N6" t="n">
-        <v>0.5600000000000001</v>
+        <v>0.59</v>
       </c>
       <c r="O6" t="n">
-        <v>0.19</v>
+        <v>0.18</v>
       </c>
       <c r="P6" t="n">
-        <v>0.25</v>
+        <v>0.24</v>
       </c>
       <c r="Q6" t="n">
-        <v>0.44</v>
+        <v>0.41</v>
       </c>
       <c r="R6" t="n">
-        <v>0.5600000000000001</v>
+        <v>0.59</v>
       </c>
     </row>
     <row r="7">
@@ -1978,55 +1978,55 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C7" t="n">
-        <v>24.643</v>
+        <v>23.482</v>
       </c>
       <c r="D7" t="n">
-        <v>34.369</v>
+        <v>33.917</v>
       </c>
       <c r="E7" t="n">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F7" t="n">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="G7" t="n">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="H7" t="n">
         <v>25</v>
       </c>
       <c r="I7" t="n">
-        <v>1.39</v>
+        <v>1.47</v>
       </c>
       <c r="J7" t="n">
-        <v>197</v>
+        <v>185</v>
       </c>
       <c r="K7" t="n">
-        <v>308</v>
+        <v>299</v>
       </c>
       <c r="L7" t="n">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="M7" t="n">
         <v>39</v>
       </c>
       <c r="N7" t="n">
-        <v>0.83</v>
+        <v>0.82</v>
       </c>
       <c r="O7" t="n">
-        <v>0.11</v>
+        <v>0.12</v>
       </c>
       <c r="P7" t="n">
         <v>0.06</v>
       </c>
       <c r="Q7" t="n">
-        <v>0.5</v>
+        <v>0.53</v>
       </c>
       <c r="R7" t="n">
-        <v>0.5</v>
+        <v>0.47</v>
       </c>
     </row>
     <row r="8">
@@ -2090,59 +2090,59 @@
     <row r="9">
       <c r="A9" s="1" t="inlineStr">
         <is>
-          <t>Werder Bremen</t>
+          <t>Eintracht Frankfurt</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C9" t="n">
-        <v>19.821</v>
+        <v>23.787</v>
       </c>
       <c r="D9" t="n">
-        <v>31.983</v>
+        <v>33.754</v>
       </c>
       <c r="E9" t="n">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="F9" t="n">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="G9" t="n">
-        <v>-6</v>
+        <v>-11</v>
       </c>
       <c r="H9" t="n">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="I9" t="n">
         <v>1</v>
       </c>
       <c r="J9" t="n">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="K9" t="n">
-        <v>302</v>
+        <v>261</v>
       </c>
       <c r="L9" t="n">
-        <v>24</v>
+        <v>32</v>
       </c>
       <c r="M9" t="n">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="N9" t="n">
-        <v>0.59</v>
+        <v>0.61</v>
       </c>
       <c r="O9" t="n">
-        <v>0.24</v>
+        <v>0.28</v>
       </c>
       <c r="P9" t="n">
-        <v>0.18</v>
+        <v>0.11</v>
       </c>
       <c r="Q9" t="n">
-        <v>0.47</v>
+        <v>0.33</v>
       </c>
       <c r="R9" t="n">
-        <v>0.53</v>
+        <v>0.67</v>
       </c>
     </row>
     <row r="10">
@@ -2206,84 +2206,84 @@
     <row r="11">
       <c r="A11" s="1" t="inlineStr">
         <is>
-          <t>Wolfsburg</t>
+          <t>Werder Bremen</t>
         </is>
       </c>
       <c r="B11" t="n">
+        <v>18</v>
+      </c>
+      <c r="C11" t="n">
+        <v>21.17</v>
+      </c>
+      <c r="D11" t="n">
+        <v>34.049</v>
+      </c>
+      <c r="E11" t="n">
+        <v>23</v>
+      </c>
+      <c r="F11" t="n">
+        <v>30</v>
+      </c>
+      <c r="G11" t="n">
+        <v>-7</v>
+      </c>
+      <c r="H11" t="n">
         <v>17</v>
       </c>
-      <c r="C11" t="n">
-        <v>20.119</v>
-      </c>
-      <c r="D11" t="n">
-        <v>29.765</v>
-      </c>
-      <c r="E11" t="n">
-        <v>18</v>
-      </c>
-      <c r="F11" t="n">
-        <v>34</v>
-      </c>
-      <c r="G11" t="n">
-        <v>-16</v>
-      </c>
-      <c r="H11" t="n">
-        <v>15</v>
-      </c>
       <c r="I11" t="n">
-        <v>0.88</v>
+        <v>0.9399999999999999</v>
       </c>
       <c r="J11" t="n">
-        <v>201</v>
+        <v>195</v>
       </c>
       <c r="K11" t="n">
-        <v>239</v>
+        <v>316</v>
       </c>
       <c r="L11" t="n">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="M11" t="n">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="N11" t="n">
-        <v>0.53</v>
+        <v>0.61</v>
       </c>
       <c r="O11" t="n">
-        <v>0.35</v>
+        <v>0.22</v>
       </c>
       <c r="P11" t="n">
-        <v>0.12</v>
+        <v>0.17</v>
       </c>
       <c r="Q11" t="n">
-        <v>0.47</v>
+        <v>0.44</v>
       </c>
       <c r="R11" t="n">
-        <v>0.53</v>
+        <v>0.5600000000000001</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="inlineStr">
         <is>
-          <t>Eintracht Frankfurt</t>
+          <t>Wolfsburg</t>
         </is>
       </c>
       <c r="B12" t="n">
         <v>17</v>
       </c>
       <c r="C12" t="n">
-        <v>22.092</v>
+        <v>20.119</v>
       </c>
       <c r="D12" t="n">
-        <v>32.906</v>
+        <v>29.765</v>
       </c>
       <c r="E12" t="n">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="F12" t="n">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="G12" t="n">
-        <v>-12</v>
+        <v>-16</v>
       </c>
       <c r="H12" t="n">
         <v>15</v>
@@ -2292,31 +2292,31 @@
         <v>0.88</v>
       </c>
       <c r="J12" t="n">
-        <v>169</v>
+        <v>201</v>
       </c>
       <c r="K12" t="n">
-        <v>245</v>
+        <v>239</v>
       </c>
       <c r="L12" t="n">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="M12" t="n">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="N12" t="n">
-        <v>0.59</v>
+        <v>0.53</v>
       </c>
       <c r="O12" t="n">
-        <v>0.29</v>
+        <v>0.35</v>
       </c>
       <c r="P12" t="n">
         <v>0.12</v>
       </c>
       <c r="Q12" t="n">
-        <v>0.29</v>
+        <v>0.47</v>
       </c>
       <c r="R12" t="n">
-        <v>0.71</v>
+        <v>0.53</v>
       </c>
     </row>
     <row r="13">
@@ -2380,44 +2380,44 @@
     <row r="14">
       <c r="A14" s="1" t="inlineStr">
         <is>
-          <t>Bochum</t>
+          <t>Augsburg</t>
         </is>
       </c>
       <c r="B14" t="n">
         <v>17</v>
       </c>
       <c r="C14" t="n">
-        <v>19.677</v>
+        <v>22.295</v>
       </c>
       <c r="D14" t="n">
-        <v>41.853</v>
+        <v>33.412</v>
       </c>
       <c r="E14" t="n">
-        <v>15</v>
+        <v>24</v>
       </c>
       <c r="F14" t="n">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="G14" t="n">
-        <v>-23</v>
+        <v>-7</v>
       </c>
       <c r="H14" t="n">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="I14" t="n">
-        <v>0.76</v>
+        <v>0.82</v>
       </c>
       <c r="J14" t="n">
-        <v>199</v>
+        <v>207</v>
       </c>
       <c r="K14" t="n">
-        <v>279</v>
+        <v>253</v>
       </c>
       <c r="L14" t="n">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="M14" t="n">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="N14" t="n">
         <v>0.59</v>
@@ -2426,13 +2426,13 @@
         <v>0.35</v>
       </c>
       <c r="P14" t="n">
-        <v>0.18</v>
+        <v>0.06</v>
       </c>
       <c r="Q14" t="n">
         <v>0.24</v>
       </c>
       <c r="R14" t="n">
-        <v>0.65</v>
+        <v>0.76</v>
       </c>
     </row>
     <row r="15">
@@ -2442,55 +2442,55 @@
         </is>
       </c>
       <c r="B15" t="n">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C15" t="n">
-        <v>18.459</v>
+        <v>17.233</v>
       </c>
       <c r="D15" t="n">
-        <v>29.897</v>
+        <v>28.565</v>
       </c>
       <c r="E15" t="n">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F15" t="n">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G15" t="n">
         <v>-15</v>
       </c>
       <c r="H15" t="n">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="I15" t="n">
-        <v>0.71</v>
+        <v>0.6899999999999999</v>
       </c>
       <c r="J15" t="n">
-        <v>195</v>
+        <v>183</v>
       </c>
       <c r="K15" t="n">
-        <v>249</v>
+        <v>234</v>
       </c>
       <c r="L15" t="n">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="M15" t="n">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="N15" t="n">
-        <v>0.41</v>
+        <v>0.38</v>
       </c>
       <c r="O15" t="n">
-        <v>0.47</v>
+        <v>0.5</v>
       </c>
       <c r="P15" t="n">
-        <v>0.18</v>
+        <v>0.19</v>
       </c>
       <c r="Q15" t="n">
-        <v>0.24</v>
+        <v>0.19</v>
       </c>
       <c r="R15" t="n">
-        <v>0.71</v>
+        <v>0.75</v>
       </c>
     </row>
     <row r="16">
@@ -2500,80 +2500,80 @@
         </is>
       </c>
       <c r="B16" t="n">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C16" t="n">
-        <v>21.71</v>
+        <v>21.322</v>
       </c>
       <c r="D16" t="n">
-        <v>30.241</v>
+        <v>28.623</v>
       </c>
       <c r="E16" t="n">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F16" t="n">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G16" t="n">
         <v>-15</v>
       </c>
       <c r="H16" t="n">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="I16" t="n">
-        <v>0.67</v>
+        <v>0.65</v>
       </c>
       <c r="J16" t="n">
-        <v>201</v>
+        <v>195</v>
       </c>
       <c r="K16" t="n">
-        <v>245</v>
+        <v>234</v>
       </c>
       <c r="L16" t="n">
         <v>29</v>
       </c>
       <c r="M16" t="n">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="N16" t="n">
-        <v>0.61</v>
+        <v>0.59</v>
       </c>
       <c r="O16" t="n">
-        <v>0.33</v>
+        <v>0.35</v>
       </c>
       <c r="P16" t="n">
-        <v>0.17</v>
+        <v>0.18</v>
       </c>
       <c r="Q16" t="n">
-        <v>0.28</v>
+        <v>0.29</v>
       </c>
       <c r="R16" t="n">
-        <v>0.61</v>
+        <v>0.59</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="1" t="inlineStr">
         <is>
-          <t>Augsburg</t>
+          <t>Borussia M.Gladbach</t>
         </is>
       </c>
       <c r="B17" t="n">
         <v>17</v>
       </c>
       <c r="C17" t="n">
-        <v>21.38</v>
+        <v>23.322</v>
       </c>
       <c r="D17" t="n">
-        <v>34.795</v>
+        <v>42.914</v>
       </c>
       <c r="E17" t="n">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="F17" t="n">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="G17" t="n">
-        <v>-15</v>
+        <v>-13</v>
       </c>
       <c r="H17" t="n">
         <v>11</v>
@@ -2582,31 +2582,31 @@
         <v>0.65</v>
       </c>
       <c r="J17" t="n">
-        <v>198</v>
+        <v>191</v>
       </c>
       <c r="K17" t="n">
-        <v>266</v>
+        <v>326</v>
       </c>
       <c r="L17" t="n">
-        <v>24</v>
+        <v>36</v>
       </c>
       <c r="M17" t="n">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="N17" t="n">
-        <v>0.65</v>
+        <v>0.82</v>
       </c>
       <c r="O17" t="n">
+        <v>0.18</v>
+      </c>
+      <c r="P17" t="n">
+        <v>0.12</v>
+      </c>
+      <c r="Q17" t="n">
         <v>0.35</v>
       </c>
-      <c r="P17" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q17" t="n">
-        <v>0.24</v>
-      </c>
       <c r="R17" t="n">
-        <v>0.76</v>
+        <v>0.53</v>
       </c>
     </row>
     <row r="18">
@@ -2670,59 +2670,59 @@
     <row r="19">
       <c r="A19" s="1" t="inlineStr">
         <is>
-          <t>Borussia M.Gladbach</t>
+          <t>Bochum</t>
         </is>
       </c>
       <c r="B19" t="n">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C19" t="n">
-        <v>23.217</v>
+        <v>17.943</v>
       </c>
       <c r="D19" t="n">
-        <v>44.092</v>
+        <v>41.268</v>
       </c>
       <c r="E19" t="n">
-        <v>25</v>
+        <v>13</v>
       </c>
       <c r="F19" t="n">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="G19" t="n">
-        <v>-16</v>
+        <v>-25</v>
       </c>
       <c r="H19" t="n">
         <v>10</v>
       </c>
       <c r="I19" t="n">
-        <v>0.59</v>
+        <v>0.62</v>
       </c>
       <c r="J19" t="n">
-        <v>184</v>
+        <v>190</v>
       </c>
       <c r="K19" t="n">
-        <v>321</v>
+        <v>268</v>
       </c>
       <c r="L19" t="n">
-        <v>35</v>
+        <v>24</v>
       </c>
       <c r="M19" t="n">
         <v>53</v>
       </c>
       <c r="N19" t="n">
-        <v>0.76</v>
+        <v>0.62</v>
       </c>
       <c r="O19" t="n">
-        <v>0.24</v>
+        <v>0.38</v>
       </c>
       <c r="P19" t="n">
         <v>0.12</v>
       </c>
       <c r="Q19" t="n">
-        <v>0.35</v>
+        <v>0.19</v>
       </c>
       <c r="R19" t="n">
-        <v>0.53</v>
+        <v>0.6899999999999999</v>
       </c>
     </row>
   </sheetData>

</xml_diff>